<commit_message>
Hoàn thành dự án Assignment Kiểm thử nâng cao C#
</commit_message>
<xml_diff>
--- a/Test_Case.xlsx
+++ b/Test_Case.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StudyProject\Assignment_KTNC(NET104 cũ)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301A45E9-DCC3-4705-B663-A579C1044854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D22FDB-BC8B-435C-92B1-AE4FFC6B3A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10215" yWindow="4500" windowWidth="20055" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestCase" sheetId="1" r:id="rId1"/>
+    <sheet name="TestReport" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="154">
   <si>
     <t>Tên dự án</t>
   </si>
@@ -444,13 +448,115 @@
   <si>
     <t>Đơn hàng được tạo đã xóa sau khi
 xác nhận thanh toán</t>
+  </si>
+  <si>
+    <t>FastFoodUITest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test đặc biệt: Lưu cookie đăng nhập Google (chạy thủ công 1 lần) </t>
+  </si>
+  <si>
+    <t>FastFoodUITest SaveCookiesOnly()</t>
+  </si>
+  <si>
+    <t>Click 'Đăng nhập với Google' và đăng nhập thủ công..."
+Trường hợp Pass: Cookie đã được lưu thành công,
+Cookie login đã được lưu!
+Trường hợp Fail:  Đăng nhập Google thất bại. Hãy thử lại.</t>
+  </si>
+  <si>
+    <t>($"{_baseUrl}/Account/Login");
+($"{c.Name}|{c.Value}|localhost|{c.Path}|{c.Expiry}");</t>
+  </si>
+  <si>
+    <t>Cookie đã được lưu thành công</t>
+  </si>
+  <si>
+    <t>FastFoodUITest  AddToCart_Should_Add_Item_And_Show
+_Success_Message()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _driver.Navigate().GoToUrl($"{_baseUrl}/Food/Index");
+_driver.Navigate().GoToUrl($"{_baseUrl}/Cart/Index");</t>
+  </si>
+  <si>
+    <t>Thêm món vào giỏ hàng</t>
+  </si>
+  <si>
+    <t>Pass:  Đã thêm món: {cartRows[0].Text}"
+Fail:  Giỏ hàng trống sau khi thêm món!</t>
+  </si>
+  <si>
+    <t>Đã đặt thêm món ăn thành công</t>
+  </si>
+  <si>
+    <t>Thanh toán đơn hàng (nhấn nút đăng nhập lại để có thể pass)</t>
+  </si>
+  <si>
+    <t>FastFoodUITest Checkout_Should_Clear_Cart_And_Show_Success_Message() LoadCookies() SaveCurrentCookies() ReloadCookiesAndRetry()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _driver.Navigate().GoToUrl($"{_baseUrl}/Cart/Index");
+ _driver.Navigate().GoToUrl($"{_baseUrl}/Cart/Checkout");</t>
+  </si>
+  <si>
+    <t>Đã thanh toán thành công nhưng nó sẽ đăng xuất
+dẫn đến timeout do đó đăng nhập lại thì sẽ tự động load 
+cookie và thoát</t>
+  </si>
+  <si>
+    <t>Pass:  Đã đến trang CompleteCheckout.
+Fail: Cookie đăng nhập đã hết hạn — tiến hành reload cookie… , Không chuyển đến trang /Cart/CompleteCheckout.</t>
+  </si>
+  <si>
+    <t>TEST REPORT</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="0"/>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Module code</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Number of  test cases</t>
+  </si>
+  <si>
+    <t>Sub total</t>
+  </si>
+  <si>
+    <t>Test coverage</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Test successful coverage</t>
+  </si>
+  <si>
+    <t>10.19.2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,8 +586,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,8 +653,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -531,12 +696,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -554,10 +855,84 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Functional Test Case v1.0" xfId="2" xr:uid="{833F27D3-85A1-4FAD-89DA-4651E84937E4}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,6 +945,34 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Export all carrier choices"/>
+      <sheetName val="Test Report"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>CR100 - Export to excel</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="D6">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -835,25 +1238,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A67" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="47.85546875" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" customWidth="1"/>
-    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="3" max="3" width="59.140625" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" customWidth="1"/>
     <col min="5" max="5" width="50.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41" customWidth="1"/>
     <col min="7" max="7" width="27.140625" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -861,7 +1264,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -869,7 +1272,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -877,13 +1280,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -909,7 +1312,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -935,7 +1338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="30">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -961,7 +1364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="30">
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
@@ -987,7 +1390,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="45">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1013,7 +1416,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
@@ -1039,7 +1442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="30">
       <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
@@ -1065,7 +1468,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="45">
       <c r="A14" s="5" t="s">
         <v>23</v>
       </c>
@@ -1091,7 +1494,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="45">
       <c r="A15" s="5" t="s">
         <v>24</v>
       </c>
@@ -1117,7 +1520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
@@ -1125,7 +1528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
@@ -1133,7 +1536,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -1141,13 +1544,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="3"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
@@ -1173,7 +1576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="30">
       <c r="A29" s="2" t="s">
         <v>14</v>
       </c>
@@ -1199,7 +1602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="30">
       <c r="A30" s="2" t="s">
         <v>17</v>
       </c>
@@ -1225,7 +1628,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
@@ -1251,7 +1654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="30">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -1277,7 +1680,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="30">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
@@ -1303,7 +1706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="30">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -1329,7 +1732,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
@@ -1355,7 +1758,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="30">
       <c r="A36" s="2" t="s">
         <v>24</v>
       </c>
@@ -1381,7 +1784,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -1389,7 +1792,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
@@ -1397,7 +1800,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
@@ -1405,13 +1808,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B42" s="3"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" s="4" t="s">
         <v>6</v>
       </c>
@@ -1437,7 +1840,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="45">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -1463,7 +1866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="75">
       <c r="A46" s="2" t="s">
         <v>17</v>
       </c>
@@ -1489,7 +1892,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="30">
       <c r="A47" s="2" t="s">
         <v>19</v>
       </c>
@@ -1515,7 +1918,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -1523,7 +1926,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
@@ -1531,7 +1934,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>2</v>
       </c>
@@ -1539,13 +1942,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B54" s="3"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8">
       <c r="A56" s="4" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1974,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="45">
       <c r="A57" s="2" t="s">
         <v>14</v>
       </c>
@@ -1597,7 +2000,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="45">
       <c r="A58" s="2" t="s">
         <v>17</v>
       </c>
@@ -1623,7 +2026,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -1631,7 +2034,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
@@ -1639,7 +2042,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>2</v>
       </c>
@@ -1647,13 +2050,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B65" s="3"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8">
       <c r="A67" s="4" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +2082,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="60">
       <c r="A68" s="2" t="s">
         <v>14</v>
       </c>
@@ -1705,7 +2108,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="60">
       <c r="A69" s="2" t="s">
         <v>17</v>
       </c>
@@ -1731,7 +2134,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="60">
       <c r="A70" s="2" t="s">
         <v>19</v>
       </c>
@@ -1757,7 +2160,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="45">
       <c r="A71" s="2" t="s">
         <v>20</v>
       </c>
@@ -1783,7 +2186,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="60">
       <c r="A72" s="2" t="s">
         <v>21</v>
       </c>
@@ -1807,6 +2210,128 @@
       </c>
       <c r="H72" s="2" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
+      <c r="A75" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="A76" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
+      <c r="A77" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
+      <c r="A78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="3"/>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="75">
+      <c r="A82" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="75">
+      <c r="A83" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="75">
+      <c r="A84" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1817,4 +2342,200 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D25BD2E-F96A-4978-8189-8D77DE204D10}">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="22.5">
+      <c r="A1" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:8" ht="22.5">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:8" ht="39">
+      <c r="A7" s="13"/>
+      <c r="B7" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="38.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21" t="str">
+        <f>'[1]Export all carrier choices'!B4</f>
+        <v>CR100 - Export to excel</v>
+      </c>
+      <c r="D8" s="22">
+        <v>28</v>
+      </c>
+      <c r="E8" s="21">
+        <v>0</v>
+      </c>
+      <c r="F8" s="21">
+        <f>'[1]Export all carrier choices'!D6</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="22">
+        <v>28</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="13"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="13"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" s="31">
+        <f>SUM(D6:D9)</f>
+        <v>28</v>
+      </c>
+      <c r="E10" s="31">
+        <f>SUM(E6:E9)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="31">
+        <f>SUM(F6:F9)</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="32">
+        <f>SUM(G6:G9)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="13"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="36">
+        <f>(D10+E10)*100/G10</f>
+        <v>100</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="37"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="36">
+        <f>D10*100/G10</f>
+        <v>100</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="G13" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>